<commit_message>
cargue excel segunda data
</commit_message>
<xml_diff>
--- a/6.05 D Tasa cambio coberturas.xlsx
+++ b/6.05 D Tasa cambio coberturas.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juan1\Desktop\GEVOLUCIONA\excel\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0BC1301-47C0-4F18-87EE-94F1F4F9EF7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10545" yWindow="105" windowWidth="13470" windowHeight="9885"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tasa cambio coberturas" sheetId="35" r:id="rId1"/>
@@ -14,7 +20,16 @@
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Tasa cambio coberturas'!$H$4:$K$63</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Tasa cambio coberturas'!$4:$6</definedName>
   </definedNames>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="181029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -511,11 +526,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -928,6 +943,45 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -946,55 +1000,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3" xfId="1"/>
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1026,7 +1041,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="1029" name="Picture 5" descr="1 logo memo color"/>
+        <xdr:cNvPr id="1029" name="Picture 5" descr="1 logo memo color">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -1072,7 +1093,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="1030" name="Picture 6" descr="logo ministerio"/>
+        <xdr:cNvPr id="1030" name="Picture 6" descr="logo ministerio">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -1149,7 +1176,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1181,9 +1208,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1215,6 +1260,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1390,42 +1453,44 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="B1:T69"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="B66" sqref="B66:L68"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="8.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="23.85546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="9.28515625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="32.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="13.5703125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="37.28515625" style="1" customWidth="1"/>
-    <col min="8" max="10" width="19.7109375" style="1" customWidth="1"/>
-    <col min="11" max="11" width="23.42578125" style="9" customWidth="1"/>
-    <col min="12" max="12" width="21.140625" style="9" customWidth="1"/>
-    <col min="13" max="16384" width="11.42578125" style="1"/>
+    <col min="1" max="1" width="5.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="8.88671875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="23.88671875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="9.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="32.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="37.33203125" style="1" customWidth="1"/>
+    <col min="8" max="10" width="19.6640625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="23.44140625" style="9" customWidth="1"/>
+    <col min="12" max="12" width="21.109375" style="9" customWidth="1"/>
+    <col min="13" max="16384" width="11.44140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:20" ht="15" customHeight="1"/>
-    <row r="2" spans="2:20" s="5" customFormat="1" ht="35.1" customHeight="1">
-      <c r="B2" s="41"/>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="41"/>
-      <c r="H2" s="41"/>
-      <c r="I2" s="41"/>
-      <c r="J2" s="41"/>
-      <c r="K2" s="41"/>
-      <c r="L2" s="41"/>
+    <row r="1" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:20" s="5" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="43"/>
+      <c r="J2" s="43"/>
+      <c r="K2" s="43"/>
+      <c r="L2" s="43"/>
       <c r="M2" s="6"/>
       <c r="N2" s="6"/>
       <c r="O2" s="6"/>
@@ -1435,18 +1500,18 @@
       <c r="S2" s="6"/>
       <c r="T2" s="6"/>
     </row>
-    <row r="3" spans="2:20" s="5" customFormat="1" ht="47.25" customHeight="1">
-      <c r="B3" s="41"/>
-      <c r="C3" s="41"/>
-      <c r="D3" s="41"/>
-      <c r="E3" s="41"/>
-      <c r="F3" s="41"/>
-      <c r="G3" s="41"/>
-      <c r="H3" s="41"/>
-      <c r="I3" s="41"/>
-      <c r="J3" s="41"/>
-      <c r="K3" s="41"/>
-      <c r="L3" s="41"/>
+    <row r="3" spans="2:20" s="5" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="43"/>
+      <c r="C3" s="43"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="43"/>
+      <c r="I3" s="43"/>
+      <c r="J3" s="43"/>
+      <c r="K3" s="43"/>
+      <c r="L3" s="43"/>
       <c r="M3" s="7"/>
       <c r="N3" s="7"/>
       <c r="O3" s="7"/>
@@ -1456,57 +1521,57 @@
       <c r="S3" s="7"/>
       <c r="T3" s="7"/>
     </row>
-    <row r="4" spans="2:20" s="2" customFormat="1" ht="63.75" customHeight="1">
-      <c r="B4" s="46" t="s">
+    <row r="4" spans="2:20" s="2" customFormat="1" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="42" t="s">
         <v>152</v>
       </c>
-      <c r="C4" s="46"/>
-      <c r="D4" s="46"/>
-      <c r="E4" s="46"/>
-      <c r="F4" s="46"/>
-      <c r="G4" s="46"/>
-      <c r="H4" s="46"/>
-      <c r="I4" s="46"/>
-      <c r="J4" s="46"/>
-      <c r="K4" s="46"/>
-      <c r="L4" s="46"/>
-    </row>
-    <row r="5" spans="2:20" s="2" customFormat="1" ht="32.25" customHeight="1">
-      <c r="B5" s="40" t="s">
+      <c r="C4" s="42"/>
+      <c r="D4" s="42"/>
+      <c r="E4" s="42"/>
+      <c r="F4" s="42"/>
+      <c r="G4" s="42"/>
+      <c r="H4" s="42"/>
+      <c r="I4" s="42"/>
+      <c r="J4" s="42"/>
+      <c r="K4" s="42"/>
+      <c r="L4" s="42"/>
+    </row>
+    <row r="5" spans="2:20" s="2" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="46" t="s">
         <v>139</v>
       </c>
-      <c r="C5" s="41" t="s">
+      <c r="C5" s="43" t="s">
         <v>143</v>
       </c>
-      <c r="D5" s="40" t="s">
+      <c r="D5" s="46" t="s">
         <v>141</v>
       </c>
-      <c r="E5" s="41" t="s">
+      <c r="E5" s="43" t="s">
         <v>142</v>
       </c>
-      <c r="F5" s="40" t="s">
+      <c r="F5" s="46" t="s">
         <v>140</v>
       </c>
-      <c r="G5" s="41" t="s">
+      <c r="G5" s="43" t="s">
         <v>144</v>
       </c>
-      <c r="H5" s="47" t="s">
+      <c r="H5" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="I5" s="47"/>
-      <c r="J5" s="47"/>
-      <c r="K5" s="47" t="s">
+      <c r="I5" s="44"/>
+      <c r="J5" s="44"/>
+      <c r="K5" s="44" t="s">
         <v>150</v>
       </c>
-      <c r="L5" s="47"/>
-    </row>
-    <row r="6" spans="2:20" ht="31.5" customHeight="1">
-      <c r="B6" s="40"/>
-      <c r="C6" s="41"/>
-      <c r="D6" s="40"/>
-      <c r="E6" s="41"/>
-      <c r="F6" s="40"/>
-      <c r="G6" s="41"/>
+      <c r="L5" s="44"/>
+    </row>
+    <row r="6" spans="2:20" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="46"/>
+      <c r="C6" s="43"/>
+      <c r="D6" s="46"/>
+      <c r="E6" s="43"/>
+      <c r="F6" s="46"/>
+      <c r="G6" s="43"/>
       <c r="H6" s="33" t="s">
         <v>147</v>
       </c>
@@ -1523,17 +1588,17 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="2:20" ht="20.25" customHeight="1">
-      <c r="B7" s="44">
+    <row r="7" spans="2:20" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="53">
         <v>1</v>
       </c>
-      <c r="C7" s="48" t="s">
+      <c r="C7" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="45">
+      <c r="D7" s="54">
         <v>1.1000000000000001</v>
       </c>
-      <c r="E7" s="54" t="s">
+      <c r="E7" s="35" t="s">
         <v>8</v>
       </c>
       <c r="F7" s="27" t="s">
@@ -1558,11 +1623,11 @@
         <v>1.79</v>
       </c>
     </row>
-    <row r="8" spans="2:20" ht="20.25" customHeight="1">
-      <c r="B8" s="43"/>
-      <c r="C8" s="49"/>
-      <c r="D8" s="42"/>
-      <c r="E8" s="51"/>
+    <row r="8" spans="2:20" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="45"/>
+      <c r="C8" s="38"/>
+      <c r="D8" s="34"/>
+      <c r="E8" s="36"/>
       <c r="F8" s="23" t="s">
         <v>11</v>
       </c>
@@ -1585,13 +1650,13 @@
         <v>9.66</v>
       </c>
     </row>
-    <row r="9" spans="2:20" ht="20.25" customHeight="1">
-      <c r="B9" s="43"/>
-      <c r="C9" s="49"/>
-      <c r="D9" s="42">
+    <row r="9" spans="2:20" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="45"/>
+      <c r="C9" s="38"/>
+      <c r="D9" s="34">
         <v>1.2</v>
       </c>
-      <c r="E9" s="51" t="s">
+      <c r="E9" s="36" t="s">
         <v>13</v>
       </c>
       <c r="F9" s="23" t="s">
@@ -1616,11 +1681,11 @@
         <v>4.9400000000000004</v>
       </c>
     </row>
-    <row r="10" spans="2:20" s="3" customFormat="1" ht="20.25" customHeight="1">
-      <c r="B10" s="43"/>
-      <c r="C10" s="49"/>
-      <c r="D10" s="42"/>
-      <c r="E10" s="51"/>
+    <row r="10" spans="2:20" s="3" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="45"/>
+      <c r="C10" s="38"/>
+      <c r="D10" s="34"/>
+      <c r="E10" s="36"/>
       <c r="F10" s="23" t="s">
         <v>16</v>
       </c>
@@ -1643,11 +1708,11 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="11" spans="2:20" ht="20.25" customHeight="1">
-      <c r="B11" s="43"/>
-      <c r="C11" s="49"/>
-      <c r="D11" s="42"/>
-      <c r="E11" s="51"/>
+    <row r="11" spans="2:20" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="45"/>
+      <c r="C11" s="38"/>
+      <c r="D11" s="34"/>
+      <c r="E11" s="36"/>
       <c r="F11" s="23" t="s">
         <v>18</v>
       </c>
@@ -1670,11 +1735,11 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="12" spans="2:20" ht="20.25" customHeight="1">
-      <c r="B12" s="43"/>
-      <c r="C12" s="49"/>
-      <c r="D12" s="42"/>
-      <c r="E12" s="51"/>
+    <row r="12" spans="2:20" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="45"/>
+      <c r="C12" s="38"/>
+      <c r="D12" s="34"/>
+      <c r="E12" s="36"/>
       <c r="F12" s="23" t="s">
         <v>20</v>
       </c>
@@ -1697,11 +1762,11 @@
         <v>-0.92</v>
       </c>
     </row>
-    <row r="13" spans="2:20" ht="20.25" customHeight="1">
-      <c r="B13" s="43"/>
-      <c r="C13" s="49"/>
-      <c r="D13" s="42"/>
-      <c r="E13" s="51"/>
+    <row r="13" spans="2:20" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="45"/>
+      <c r="C13" s="38"/>
+      <c r="D13" s="34"/>
+      <c r="E13" s="36"/>
       <c r="F13" s="23" t="s">
         <v>22</v>
       </c>
@@ -1724,13 +1789,13 @@
         <v>26.73</v>
       </c>
     </row>
-    <row r="14" spans="2:20" ht="20.25" customHeight="1">
-      <c r="B14" s="43"/>
-      <c r="C14" s="49"/>
-      <c r="D14" s="42">
+    <row r="14" spans="2:20" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="45"/>
+      <c r="C14" s="38"/>
+      <c r="D14" s="34">
         <v>1.3</v>
       </c>
-      <c r="E14" s="51" t="s">
+      <c r="E14" s="36" t="s">
         <v>24</v>
       </c>
       <c r="F14" s="23" t="s">
@@ -1755,11 +1820,11 @@
         <v>7.99</v>
       </c>
     </row>
-    <row r="15" spans="2:20" ht="20.25" customHeight="1">
-      <c r="B15" s="43"/>
-      <c r="C15" s="49"/>
-      <c r="D15" s="42"/>
-      <c r="E15" s="51"/>
+    <row r="15" spans="2:20" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="45"/>
+      <c r="C15" s="38"/>
+      <c r="D15" s="34"/>
+      <c r="E15" s="36"/>
       <c r="F15" s="23" t="s">
         <v>27</v>
       </c>
@@ -1782,13 +1847,13 @@
         <v>168.19</v>
       </c>
     </row>
-    <row r="16" spans="2:20" ht="20.25" customHeight="1">
-      <c r="B16" s="43"/>
-      <c r="C16" s="49"/>
-      <c r="D16" s="42">
+    <row r="16" spans="2:20" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="45"/>
+      <c r="C16" s="38"/>
+      <c r="D16" s="34">
         <v>1.4</v>
       </c>
-      <c r="E16" s="51" t="s">
+      <c r="E16" s="36" t="s">
         <v>29</v>
       </c>
       <c r="F16" s="23" t="s">
@@ -1813,11 +1878,11 @@
         <v>15.4</v>
       </c>
     </row>
-    <row r="17" spans="2:12" ht="20.25" customHeight="1">
-      <c r="B17" s="43"/>
-      <c r="C17" s="49"/>
-      <c r="D17" s="42"/>
-      <c r="E17" s="51"/>
+    <row r="17" spans="2:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="45"/>
+      <c r="C17" s="38"/>
+      <c r="D17" s="34"/>
+      <c r="E17" s="36"/>
       <c r="F17" s="23" t="s">
         <v>32</v>
       </c>
@@ -1840,17 +1905,17 @@
         <v>12.82</v>
       </c>
     </row>
-    <row r="18" spans="2:12" ht="20.25" customHeight="1">
-      <c r="B18" s="43">
+    <row r="18" spans="2:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="45">
         <v>2</v>
       </c>
-      <c r="C18" s="49" t="s">
+      <c r="C18" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="D18" s="42">
+      <c r="D18" s="34">
         <v>2.1</v>
       </c>
-      <c r="E18" s="51" t="s">
+      <c r="E18" s="36" t="s">
         <v>35</v>
       </c>
       <c r="F18" s="23" t="s">
@@ -1875,11 +1940,11 @@
         <v>-8.66</v>
       </c>
     </row>
-    <row r="19" spans="2:12" ht="20.25" customHeight="1">
-      <c r="B19" s="43"/>
-      <c r="C19" s="49"/>
-      <c r="D19" s="42"/>
-      <c r="E19" s="51"/>
+    <row r="19" spans="2:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="45"/>
+      <c r="C19" s="38"/>
+      <c r="D19" s="34"/>
+      <c r="E19" s="36"/>
       <c r="F19" s="23" t="s">
         <v>38</v>
       </c>
@@ -1902,11 +1967,11 @@
         <v>1.02</v>
       </c>
     </row>
-    <row r="20" spans="2:12" ht="20.25" customHeight="1">
-      <c r="B20" s="43"/>
-      <c r="C20" s="49"/>
-      <c r="D20" s="42"/>
-      <c r="E20" s="51"/>
+    <row r="20" spans="2:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="45"/>
+      <c r="C20" s="38"/>
+      <c r="D20" s="34"/>
+      <c r="E20" s="36"/>
       <c r="F20" s="23" t="s">
         <v>40</v>
       </c>
@@ -1929,11 +1994,11 @@
         <v>59.72</v>
       </c>
     </row>
-    <row r="21" spans="2:12" ht="20.25" customHeight="1">
-      <c r="B21" s="43"/>
-      <c r="C21" s="49"/>
-      <c r="D21" s="42"/>
-      <c r="E21" s="51"/>
+    <row r="21" spans="2:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="45"/>
+      <c r="C21" s="38"/>
+      <c r="D21" s="34"/>
+      <c r="E21" s="36"/>
       <c r="F21" s="23" t="s">
         <v>42</v>
       </c>
@@ -1956,11 +2021,11 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="22" spans="2:12" ht="20.25" customHeight="1">
-      <c r="B22" s="43"/>
-      <c r="C22" s="49"/>
-      <c r="D22" s="42"/>
-      <c r="E22" s="51"/>
+    <row r="22" spans="2:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="45"/>
+      <c r="C22" s="38"/>
+      <c r="D22" s="34"/>
+      <c r="E22" s="36"/>
       <c r="F22" s="23" t="s">
         <v>44</v>
       </c>
@@ -1983,13 +2048,13 @@
         <v>-4.04</v>
       </c>
     </row>
-    <row r="23" spans="2:12" ht="20.25" customHeight="1">
-      <c r="B23" s="43"/>
-      <c r="C23" s="49"/>
-      <c r="D23" s="42">
+    <row r="23" spans="2:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="45"/>
+      <c r="C23" s="38"/>
+      <c r="D23" s="34">
         <v>2.2000000000000002</v>
       </c>
-      <c r="E23" s="51" t="s">
+      <c r="E23" s="36" t="s">
         <v>46</v>
       </c>
       <c r="F23" s="23" t="s">
@@ -2014,11 +2079,11 @@
         <v>3.01</v>
       </c>
     </row>
-    <row r="24" spans="2:12" ht="20.25" customHeight="1">
-      <c r="B24" s="43"/>
-      <c r="C24" s="49"/>
-      <c r="D24" s="42"/>
-      <c r="E24" s="51"/>
+    <row r="24" spans="2:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="45"/>
+      <c r="C24" s="38"/>
+      <c r="D24" s="34"/>
+      <c r="E24" s="36"/>
       <c r="F24" s="23" t="s">
         <v>49</v>
       </c>
@@ -2041,11 +2106,11 @@
         <v>1.19</v>
       </c>
     </row>
-    <row r="25" spans="2:12" ht="20.25" customHeight="1">
-      <c r="B25" s="43"/>
-      <c r="C25" s="49"/>
-      <c r="D25" s="42"/>
-      <c r="E25" s="51"/>
+    <row r="25" spans="2:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="45"/>
+      <c r="C25" s="38"/>
+      <c r="D25" s="34"/>
+      <c r="E25" s="36"/>
       <c r="F25" s="23" t="s">
         <v>51</v>
       </c>
@@ -2068,11 +2133,11 @@
         <v>11.87</v>
       </c>
     </row>
-    <row r="26" spans="2:12" s="4" customFormat="1" ht="20.25" customHeight="1">
-      <c r="B26" s="43"/>
-      <c r="C26" s="49"/>
-      <c r="D26" s="42"/>
-      <c r="E26" s="51"/>
+    <row r="26" spans="2:12" s="4" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="45"/>
+      <c r="C26" s="38"/>
+      <c r="D26" s="34"/>
+      <c r="E26" s="36"/>
       <c r="F26" s="23" t="s">
         <v>53</v>
       </c>
@@ -2095,11 +2160,11 @@
         <v>36.229999999999997</v>
       </c>
     </row>
-    <row r="27" spans="2:12" ht="20.25" customHeight="1">
-      <c r="B27" s="43"/>
-      <c r="C27" s="49"/>
-      <c r="D27" s="42"/>
-      <c r="E27" s="51"/>
+    <row r="27" spans="2:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="45"/>
+      <c r="C27" s="38"/>
+      <c r="D27" s="34"/>
+      <c r="E27" s="36"/>
       <c r="F27" s="23" t="s">
         <v>55</v>
       </c>
@@ -2122,13 +2187,13 @@
         <v>2.88</v>
       </c>
     </row>
-    <row r="28" spans="2:12" ht="20.25" customHeight="1">
-      <c r="B28" s="43"/>
-      <c r="C28" s="49"/>
-      <c r="D28" s="42">
+    <row r="28" spans="2:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="45"/>
+      <c r="C28" s="38"/>
+      <c r="D28" s="34">
         <v>2.2999999999999998</v>
       </c>
-      <c r="E28" s="51" t="s">
+      <c r="E28" s="36" t="s">
         <v>57</v>
       </c>
       <c r="F28" s="23" t="s">
@@ -2153,11 +2218,11 @@
         <v>2.3199999999999998</v>
       </c>
     </row>
-    <row r="29" spans="2:12" ht="20.25" customHeight="1">
-      <c r="B29" s="43"/>
-      <c r="C29" s="49"/>
-      <c r="D29" s="42"/>
-      <c r="E29" s="51"/>
+    <row r="29" spans="2:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="45"/>
+      <c r="C29" s="38"/>
+      <c r="D29" s="34"/>
+      <c r="E29" s="36"/>
       <c r="F29" s="23" t="s">
         <v>60</v>
       </c>
@@ -2180,11 +2245,11 @@
         <v>-0.25</v>
       </c>
     </row>
-    <row r="30" spans="2:12" ht="20.25" customHeight="1">
-      <c r="B30" s="43"/>
-      <c r="C30" s="49"/>
-      <c r="D30" s="42"/>
-      <c r="E30" s="51"/>
+    <row r="30" spans="2:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="45"/>
+      <c r="C30" s="38"/>
+      <c r="D30" s="34"/>
+      <c r="E30" s="36"/>
       <c r="F30" s="23" t="s">
         <v>62</v>
       </c>
@@ -2207,13 +2272,13 @@
         <v>0.21</v>
       </c>
     </row>
-    <row r="31" spans="2:12" ht="20.25" customHeight="1">
-      <c r="B31" s="43"/>
-      <c r="C31" s="49"/>
-      <c r="D31" s="42">
+    <row r="31" spans="2:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="45"/>
+      <c r="C31" s="38"/>
+      <c r="D31" s="34">
         <v>2.4</v>
       </c>
-      <c r="E31" s="51" t="s">
+      <c r="E31" s="36" t="s">
         <v>64</v>
       </c>
       <c r="F31" s="23" t="s">
@@ -2238,11 +2303,11 @@
         <v>7.37</v>
       </c>
     </row>
-    <row r="32" spans="2:12" ht="20.25" customHeight="1">
-      <c r="B32" s="43"/>
-      <c r="C32" s="49"/>
-      <c r="D32" s="42"/>
-      <c r="E32" s="51"/>
+    <row r="32" spans="2:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="45"/>
+      <c r="C32" s="38"/>
+      <c r="D32" s="34"/>
+      <c r="E32" s="36"/>
       <c r="F32" s="23" t="s">
         <v>67</v>
       </c>
@@ -2265,11 +2330,11 @@
         <v>-1.35</v>
       </c>
     </row>
-    <row r="33" spans="2:12" ht="33.75" customHeight="1">
-      <c r="B33" s="43"/>
-      <c r="C33" s="49"/>
-      <c r="D33" s="42"/>
-      <c r="E33" s="51"/>
+    <row r="33" spans="2:12" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="45"/>
+      <c r="C33" s="38"/>
+      <c r="D33" s="34"/>
+      <c r="E33" s="36"/>
       <c r="F33" s="23" t="s">
         <v>69</v>
       </c>
@@ -2292,11 +2357,11 @@
         <v>-3.24</v>
       </c>
     </row>
-    <row r="34" spans="2:12" ht="20.25" customHeight="1">
-      <c r="B34" s="43"/>
-      <c r="C34" s="49"/>
-      <c r="D34" s="42"/>
-      <c r="E34" s="51"/>
+    <row r="34" spans="2:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="45"/>
+      <c r="C34" s="38"/>
+      <c r="D34" s="34"/>
+      <c r="E34" s="36"/>
       <c r="F34" s="23" t="s">
         <v>71</v>
       </c>
@@ -2319,11 +2384,11 @@
         <v>-1.69</v>
       </c>
     </row>
-    <row r="35" spans="2:12" ht="20.25" customHeight="1">
-      <c r="B35" s="43"/>
-      <c r="C35" s="49"/>
-      <c r="D35" s="42"/>
-      <c r="E35" s="51"/>
+    <row r="35" spans="2:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B35" s="45"/>
+      <c r="C35" s="38"/>
+      <c r="D35" s="34"/>
+      <c r="E35" s="36"/>
       <c r="F35" s="23" t="s">
         <v>73</v>
       </c>
@@ -2346,17 +2411,17 @@
         <v>4.24</v>
       </c>
     </row>
-    <row r="36" spans="2:12" ht="20.25" customHeight="1">
-      <c r="B36" s="43">
+    <row r="36" spans="2:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B36" s="45">
         <v>3</v>
       </c>
-      <c r="C36" s="52" t="s">
+      <c r="C36" s="40" t="s">
         <v>75</v>
       </c>
-      <c r="D36" s="42">
+      <c r="D36" s="34">
         <v>3.1</v>
       </c>
-      <c r="E36" s="51" t="s">
+      <c r="E36" s="36" t="s">
         <v>76</v>
       </c>
       <c r="F36" s="23" t="s">
@@ -2381,11 +2446,11 @@
         <v>-0.45</v>
       </c>
     </row>
-    <row r="37" spans="2:12" ht="20.25" customHeight="1">
-      <c r="B37" s="43"/>
-      <c r="C37" s="53"/>
-      <c r="D37" s="42"/>
-      <c r="E37" s="51"/>
+    <row r="37" spans="2:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B37" s="45"/>
+      <c r="C37" s="41"/>
+      <c r="D37" s="34"/>
+      <c r="E37" s="36"/>
       <c r="F37" s="23" t="s">
         <v>79</v>
       </c>
@@ -2408,11 +2473,11 @@
         <v>8.0399999999999991</v>
       </c>
     </row>
-    <row r="38" spans="2:12" ht="20.25" customHeight="1">
-      <c r="B38" s="43"/>
-      <c r="C38" s="53"/>
-      <c r="D38" s="42"/>
-      <c r="E38" s="51"/>
+    <row r="38" spans="2:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B38" s="45"/>
+      <c r="C38" s="41"/>
+      <c r="D38" s="34"/>
+      <c r="E38" s="36"/>
       <c r="F38" s="23" t="s">
         <v>81</v>
       </c>
@@ -2435,11 +2500,11 @@
         <v>1.72</v>
       </c>
     </row>
-    <row r="39" spans="2:12" ht="20.25" customHeight="1">
-      <c r="B39" s="43"/>
-      <c r="C39" s="53"/>
-      <c r="D39" s="42"/>
-      <c r="E39" s="51"/>
+    <row r="39" spans="2:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B39" s="45"/>
+      <c r="C39" s="41"/>
+      <c r="D39" s="34"/>
+      <c r="E39" s="36"/>
       <c r="F39" s="23" t="s">
         <v>83</v>
       </c>
@@ -2462,11 +2527,11 @@
         <v>2.37</v>
       </c>
     </row>
-    <row r="40" spans="2:12" ht="20.25" customHeight="1">
-      <c r="B40" s="43"/>
-      <c r="C40" s="53"/>
-      <c r="D40" s="42"/>
-      <c r="E40" s="51"/>
+    <row r="40" spans="2:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B40" s="45"/>
+      <c r="C40" s="41"/>
+      <c r="D40" s="34"/>
+      <c r="E40" s="36"/>
       <c r="F40" s="23" t="s">
         <v>85</v>
       </c>
@@ -2489,13 +2554,13 @@
         <v>10.34</v>
       </c>
     </row>
-    <row r="41" spans="2:12" ht="20.25" customHeight="1">
-      <c r="B41" s="43"/>
-      <c r="C41" s="53"/>
-      <c r="D41" s="42">
+    <row r="41" spans="2:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B41" s="45"/>
+      <c r="C41" s="41"/>
+      <c r="D41" s="34">
         <v>3.2</v>
       </c>
-      <c r="E41" s="51" t="s">
+      <c r="E41" s="36" t="s">
         <v>87</v>
       </c>
       <c r="F41" s="23" t="s">
@@ -2520,11 +2585,11 @@
         <v>0.13</v>
       </c>
     </row>
-    <row r="42" spans="2:12" ht="20.25" customHeight="1">
-      <c r="B42" s="43"/>
-      <c r="C42" s="53"/>
-      <c r="D42" s="42"/>
-      <c r="E42" s="51"/>
+    <row r="42" spans="2:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B42" s="45"/>
+      <c r="C42" s="41"/>
+      <c r="D42" s="34"/>
+      <c r="E42" s="36"/>
       <c r="F42" s="23" t="s">
         <v>90</v>
       </c>
@@ -2547,11 +2612,11 @@
         <v>-4.46</v>
       </c>
     </row>
-    <row r="43" spans="2:12" ht="20.25" customHeight="1">
-      <c r="B43" s="43"/>
-      <c r="C43" s="53"/>
-      <c r="D43" s="42"/>
-      <c r="E43" s="51"/>
+    <row r="43" spans="2:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B43" s="45"/>
+      <c r="C43" s="41"/>
+      <c r="D43" s="34"/>
+      <c r="E43" s="36"/>
       <c r="F43" s="23" t="s">
         <v>92</v>
       </c>
@@ -2574,13 +2639,13 @@
         <v>8.18</v>
       </c>
     </row>
-    <row r="44" spans="2:12" ht="20.25" customHeight="1">
-      <c r="B44" s="43"/>
-      <c r="C44" s="53"/>
-      <c r="D44" s="42">
+    <row r="44" spans="2:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B44" s="45"/>
+      <c r="C44" s="41"/>
+      <c r="D44" s="34">
         <v>3.3</v>
       </c>
-      <c r="E44" s="51" t="s">
+      <c r="E44" s="36" t="s">
         <v>94</v>
       </c>
       <c r="F44" s="23" t="s">
@@ -2605,11 +2670,11 @@
         <v>-2.15</v>
       </c>
     </row>
-    <row r="45" spans="2:12" ht="20.25" customHeight="1">
-      <c r="B45" s="43"/>
-      <c r="C45" s="53"/>
-      <c r="D45" s="42"/>
-      <c r="E45" s="51"/>
+    <row r="45" spans="2:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B45" s="45"/>
+      <c r="C45" s="41"/>
+      <c r="D45" s="34"/>
+      <c r="E45" s="36"/>
       <c r="F45" s="23" t="s">
         <v>97</v>
       </c>
@@ -2632,11 +2697,11 @@
         <v>-0.28999999999999998</v>
       </c>
     </row>
-    <row r="46" spans="2:12" ht="20.25" customHeight="1">
-      <c r="B46" s="43"/>
-      <c r="C46" s="53"/>
-      <c r="D46" s="42"/>
-      <c r="E46" s="51"/>
+    <row r="46" spans="2:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B46" s="45"/>
+      <c r="C46" s="41"/>
+      <c r="D46" s="34"/>
+      <c r="E46" s="36"/>
       <c r="F46" s="23" t="s">
         <v>99</v>
       </c>
@@ -2659,11 +2724,11 @@
         <v>-2.61</v>
       </c>
     </row>
-    <row r="47" spans="2:12" ht="20.25" customHeight="1">
-      <c r="B47" s="43"/>
-      <c r="C47" s="53"/>
-      <c r="D47" s="42"/>
-      <c r="E47" s="51"/>
+    <row r="47" spans="2:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B47" s="45"/>
+      <c r="C47" s="41"/>
+      <c r="D47" s="34"/>
+      <c r="E47" s="36"/>
       <c r="F47" s="23" t="s">
         <v>101</v>
       </c>
@@ -2686,11 +2751,11 @@
         <v>-6.64</v>
       </c>
     </row>
-    <row r="48" spans="2:12" ht="20.25" customHeight="1">
-      <c r="B48" s="43"/>
-      <c r="C48" s="54"/>
-      <c r="D48" s="42"/>
-      <c r="E48" s="51"/>
+    <row r="48" spans="2:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B48" s="45"/>
+      <c r="C48" s="35"/>
+      <c r="D48" s="34"/>
+      <c r="E48" s="36"/>
       <c r="F48" s="23" t="s">
         <v>103</v>
       </c>
@@ -2713,17 +2778,17 @@
         <v>-1.1000000000000001</v>
       </c>
     </row>
-    <row r="49" spans="2:12" ht="20.25" customHeight="1">
-      <c r="B49" s="43">
+    <row r="49" spans="2:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B49" s="45">
         <v>4</v>
       </c>
-      <c r="C49" s="50" t="s">
+      <c r="C49" s="39" t="s">
         <v>105</v>
       </c>
-      <c r="D49" s="42">
+      <c r="D49" s="34">
         <v>4.0999999999999996</v>
       </c>
-      <c r="E49" s="51" t="s">
+      <c r="E49" s="36" t="s">
         <v>106</v>
       </c>
       <c r="F49" s="23" t="s">
@@ -2748,11 +2813,11 @@
         <v>-2.42</v>
       </c>
     </row>
-    <row r="50" spans="2:12" ht="23.25" customHeight="1">
-      <c r="B50" s="43"/>
-      <c r="C50" s="50"/>
-      <c r="D50" s="42"/>
-      <c r="E50" s="51"/>
+    <row r="50" spans="2:12" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B50" s="45"/>
+      <c r="C50" s="39"/>
+      <c r="D50" s="34"/>
+      <c r="E50" s="36"/>
       <c r="F50" s="23" t="s">
         <v>109</v>
       </c>
@@ -2775,11 +2840,11 @@
         <v>11.32</v>
       </c>
     </row>
-    <row r="51" spans="2:12" ht="28.5" customHeight="1">
-      <c r="B51" s="43"/>
-      <c r="C51" s="50"/>
-      <c r="D51" s="42"/>
-      <c r="E51" s="51"/>
+    <row r="51" spans="2:12" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B51" s="45"/>
+      <c r="C51" s="39"/>
+      <c r="D51" s="34"/>
+      <c r="E51" s="36"/>
       <c r="F51" s="23" t="s">
         <v>111</v>
       </c>
@@ -2802,13 +2867,13 @@
         <v>-4.9800000000000004</v>
       </c>
     </row>
-    <row r="52" spans="2:12" ht="20.25" customHeight="1">
-      <c r="B52" s="43"/>
-      <c r="C52" s="50"/>
-      <c r="D52" s="42">
+    <row r="52" spans="2:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B52" s="45"/>
+      <c r="C52" s="39"/>
+      <c r="D52" s="34">
         <v>4.2</v>
       </c>
-      <c r="E52" s="51" t="s">
+      <c r="E52" s="36" t="s">
         <v>113</v>
       </c>
       <c r="F52" s="23" t="s">
@@ -2833,11 +2898,11 @@
         <v>5.8</v>
       </c>
     </row>
-    <row r="53" spans="2:12" ht="20.25" customHeight="1">
-      <c r="B53" s="43"/>
-      <c r="C53" s="50"/>
-      <c r="D53" s="42"/>
-      <c r="E53" s="51"/>
+    <row r="53" spans="2:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B53" s="45"/>
+      <c r="C53" s="39"/>
+      <c r="D53" s="34"/>
+      <c r="E53" s="36"/>
       <c r="F53" s="23" t="s">
         <v>116</v>
       </c>
@@ -2860,11 +2925,11 @@
         <v>-0.78</v>
       </c>
     </row>
-    <row r="54" spans="2:12" ht="20.25" customHeight="1">
-      <c r="B54" s="43"/>
-      <c r="C54" s="50"/>
-      <c r="D54" s="42"/>
-      <c r="E54" s="51"/>
+    <row r="54" spans="2:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B54" s="45"/>
+      <c r="C54" s="39"/>
+      <c r="D54" s="34"/>
+      <c r="E54" s="36"/>
       <c r="F54" s="23" t="s">
         <v>118</v>
       </c>
@@ -2887,17 +2952,17 @@
         <v>-24.99</v>
       </c>
     </row>
-    <row r="55" spans="2:12" ht="20.25" customHeight="1">
-      <c r="B55" s="43">
+    <row r="55" spans="2:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B55" s="45">
         <v>5</v>
       </c>
-      <c r="C55" s="50" t="s">
+      <c r="C55" s="39" t="s">
         <v>120</v>
       </c>
-      <c r="D55" s="42">
+      <c r="D55" s="34">
         <v>5.0999999999999996</v>
       </c>
-      <c r="E55" s="51" t="s">
+      <c r="E55" s="36" t="s">
         <v>121</v>
       </c>
       <c r="F55" s="23" t="s">
@@ -2922,11 +2987,11 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="56" spans="2:12" ht="20.25" customHeight="1">
-      <c r="B56" s="43"/>
-      <c r="C56" s="50"/>
-      <c r="D56" s="42"/>
-      <c r="E56" s="51"/>
+    <row r="56" spans="2:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B56" s="45"/>
+      <c r="C56" s="39"/>
+      <c r="D56" s="34"/>
+      <c r="E56" s="36"/>
       <c r="F56" s="23" t="s">
         <v>124</v>
       </c>
@@ -2949,11 +3014,11 @@
         <v>-0.21</v>
       </c>
     </row>
-    <row r="57" spans="2:12" ht="20.25" customHeight="1">
-      <c r="B57" s="43"/>
-      <c r="C57" s="50"/>
-      <c r="D57" s="42"/>
-      <c r="E57" s="51"/>
+    <row r="57" spans="2:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B57" s="45"/>
+      <c r="C57" s="39"/>
+      <c r="D57" s="34"/>
+      <c r="E57" s="36"/>
       <c r="F57" s="23" t="s">
         <v>126</v>
       </c>
@@ -2976,11 +3041,11 @@
         <v>1.32</v>
       </c>
     </row>
-    <row r="58" spans="2:12" ht="20.25" customHeight="1">
-      <c r="B58" s="43"/>
-      <c r="C58" s="50"/>
-      <c r="D58" s="42"/>
-      <c r="E58" s="51"/>
+    <row r="58" spans="2:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B58" s="45"/>
+      <c r="C58" s="39"/>
+      <c r="D58" s="34"/>
+      <c r="E58" s="36"/>
       <c r="F58" s="23" t="s">
         <v>128</v>
       </c>
@@ -3003,13 +3068,13 @@
         <v>0.36</v>
       </c>
     </row>
-    <row r="59" spans="2:12" ht="20.25" customHeight="1">
-      <c r="B59" s="43"/>
-      <c r="C59" s="50"/>
-      <c r="D59" s="42">
+    <row r="59" spans="2:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B59" s="45"/>
+      <c r="C59" s="39"/>
+      <c r="D59" s="34">
         <v>5.2</v>
       </c>
-      <c r="E59" s="51" t="s">
+      <c r="E59" s="36" t="s">
         <v>130</v>
       </c>
       <c r="F59" s="23" t="s">
@@ -3034,11 +3099,11 @@
         <v>-2.93</v>
       </c>
     </row>
-    <row r="60" spans="2:12" ht="20.25" customHeight="1">
-      <c r="B60" s="43"/>
-      <c r="C60" s="50"/>
-      <c r="D60" s="42"/>
-      <c r="E60" s="51"/>
+    <row r="60" spans="2:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B60" s="45"/>
+      <c r="C60" s="39"/>
+      <c r="D60" s="34"/>
+      <c r="E60" s="36"/>
       <c r="F60" s="23" t="s">
         <v>133</v>
       </c>
@@ -3061,11 +3126,11 @@
         <v>-17.88</v>
       </c>
     </row>
-    <row r="61" spans="2:12" ht="20.25" customHeight="1">
-      <c r="B61" s="43"/>
-      <c r="C61" s="50"/>
-      <c r="D61" s="42"/>
-      <c r="E61" s="51"/>
+    <row r="61" spans="2:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B61" s="45"/>
+      <c r="C61" s="39"/>
+      <c r="D61" s="34"/>
+      <c r="E61" s="36"/>
       <c r="F61" s="23" t="s">
         <v>135</v>
       </c>
@@ -3088,7 +3153,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="2:12" ht="20.25" customHeight="1">
+    <row r="62" spans="2:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B62" s="25">
         <v>9</v>
       </c>
@@ -3123,15 +3188,15 @@
         <v>-36.83</v>
       </c>
     </row>
-    <row r="63" spans="2:12" ht="30" customHeight="1">
-      <c r="B63" s="34" t="s">
+    <row r="63" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B63" s="47" t="s">
         <v>145</v>
       </c>
-      <c r="C63" s="35"/>
-      <c r="D63" s="35"/>
-      <c r="E63" s="35"/>
-      <c r="F63" s="35"/>
-      <c r="G63" s="36"/>
+      <c r="C63" s="48"/>
+      <c r="D63" s="48"/>
+      <c r="E63" s="48"/>
+      <c r="F63" s="48"/>
+      <c r="G63" s="49"/>
       <c r="H63" s="22">
         <f>SUM(H7:H62)</f>
         <v>113988009.87859549</v>
@@ -3147,70 +3212,70 @@
       <c r="K63" s="30"/>
       <c r="L63" s="31"/>
     </row>
-    <row r="65" spans="2:12" ht="44.25" customHeight="1">
-      <c r="B65" s="37" t="s">
+    <row r="65" spans="2:12" ht="44.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B65" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="C65" s="37"/>
-      <c r="D65" s="37"/>
-      <c r="E65" s="37"/>
-      <c r="F65" s="37"/>
-      <c r="G65" s="37"/>
-      <c r="H65" s="37"/>
-      <c r="I65" s="37"/>
-      <c r="J65" s="37"/>
-      <c r="K65" s="37"/>
-      <c r="L65" s="37"/>
-    </row>
-    <row r="66" spans="2:12" ht="45" customHeight="1">
-      <c r="B66" s="38" t="s">
+      <c r="C65" s="50"/>
+      <c r="D65" s="50"/>
+      <c r="E65" s="50"/>
+      <c r="F65" s="50"/>
+      <c r="G65" s="50"/>
+      <c r="H65" s="50"/>
+      <c r="I65" s="50"/>
+      <c r="J65" s="50"/>
+      <c r="K65" s="50"/>
+      <c r="L65" s="50"/>
+    </row>
+    <row r="66" spans="2:12" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B66" s="51" t="s">
         <v>151</v>
       </c>
-      <c r="C66" s="38"/>
-      <c r="D66" s="38"/>
-      <c r="E66" s="38"/>
-      <c r="F66" s="38"/>
-      <c r="G66" s="38"/>
-      <c r="H66" s="38"/>
-      <c r="I66" s="38"/>
-      <c r="J66" s="38"/>
-      <c r="K66" s="38"/>
-      <c r="L66" s="38"/>
-    </row>
-    <row r="67" spans="2:12" ht="29.25" customHeight="1">
-      <c r="B67" s="38"/>
-      <c r="C67" s="38"/>
-      <c r="D67" s="38"/>
-      <c r="E67" s="38"/>
-      <c r="F67" s="38"/>
-      <c r="G67" s="38"/>
-      <c r="H67" s="38"/>
-      <c r="I67" s="38"/>
-      <c r="J67" s="38"/>
-      <c r="K67" s="38"/>
-      <c r="L67" s="38"/>
-    </row>
-    <row r="68" spans="2:12" ht="78.75" customHeight="1">
-      <c r="B68" s="38"/>
-      <c r="C68" s="38"/>
-      <c r="D68" s="38"/>
-      <c r="E68" s="38"/>
-      <c r="F68" s="38"/>
-      <c r="G68" s="38"/>
-      <c r="H68" s="38"/>
-      <c r="I68" s="38"/>
-      <c r="J68" s="38"/>
-      <c r="K68" s="38"/>
-      <c r="L68" s="38"/>
-    </row>
-    <row r="69" spans="2:12" ht="36" customHeight="1">
-      <c r="B69" s="39" t="s">
+      <c r="C66" s="51"/>
+      <c r="D66" s="51"/>
+      <c r="E66" s="51"/>
+      <c r="F66" s="51"/>
+      <c r="G66" s="51"/>
+      <c r="H66" s="51"/>
+      <c r="I66" s="51"/>
+      <c r="J66" s="51"/>
+      <c r="K66" s="51"/>
+      <c r="L66" s="51"/>
+    </row>
+    <row r="67" spans="2:12" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B67" s="51"/>
+      <c r="C67" s="51"/>
+      <c r="D67" s="51"/>
+      <c r="E67" s="51"/>
+      <c r="F67" s="51"/>
+      <c r="G67" s="51"/>
+      <c r="H67" s="51"/>
+      <c r="I67" s="51"/>
+      <c r="J67" s="51"/>
+      <c r="K67" s="51"/>
+      <c r="L67" s="51"/>
+    </row>
+    <row r="68" spans="2:12" ht="165" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B68" s="51"/>
+      <c r="C68" s="51"/>
+      <c r="D68" s="51"/>
+      <c r="E68" s="51"/>
+      <c r="F68" s="51"/>
+      <c r="G68" s="51"/>
+      <c r="H68" s="51"/>
+      <c r="I68" s="51"/>
+      <c r="J68" s="51"/>
+      <c r="K68" s="51"/>
+      <c r="L68" s="51"/>
+    </row>
+    <row r="69" spans="2:12" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B69" s="52" t="s">
         <v>146</v>
       </c>
-      <c r="C69" s="39"/>
-      <c r="D69" s="39"/>
-      <c r="E69" s="39"/>
-      <c r="F69" s="39"/>
+      <c r="C69" s="52"/>
+      <c r="D69" s="52"/>
+      <c r="E69" s="52"/>
+      <c r="F69" s="52"/>
       <c r="G69" s="13"/>
       <c r="H69" s="32"/>
       <c r="I69" s="32"/>
@@ -3220,12 +3285,38 @@
     </row>
   </sheetData>
   <mergeCells count="54">
-    <mergeCell ref="D28:D30"/>
-    <mergeCell ref="D31:D35"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="E9:E13"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="B63:G63"/>
+    <mergeCell ref="B65:L65"/>
+    <mergeCell ref="B66:L68"/>
+    <mergeCell ref="B69:F69"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D52:D54"/>
+    <mergeCell ref="B18:B35"/>
+    <mergeCell ref="D18:D22"/>
+    <mergeCell ref="D23:D27"/>
+    <mergeCell ref="B7:B17"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="D9:D13"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="B4:L4"/>
+    <mergeCell ref="B2:L3"/>
+    <mergeCell ref="H5:J5"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="B55:B61"/>
+    <mergeCell ref="D55:D58"/>
+    <mergeCell ref="D59:D61"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="B36:B48"/>
+    <mergeCell ref="D36:D40"/>
+    <mergeCell ref="D41:D43"/>
+    <mergeCell ref="D44:D48"/>
+    <mergeCell ref="B49:B54"/>
+    <mergeCell ref="D49:D51"/>
     <mergeCell ref="C7:C17"/>
     <mergeCell ref="C55:C61"/>
     <mergeCell ref="E55:E58"/>
@@ -3242,38 +3333,12 @@
     <mergeCell ref="E23:E27"/>
     <mergeCell ref="E28:E30"/>
     <mergeCell ref="E31:E35"/>
-    <mergeCell ref="B4:L4"/>
-    <mergeCell ref="B2:L3"/>
-    <mergeCell ref="H5:J5"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="B55:B61"/>
-    <mergeCell ref="D55:D58"/>
-    <mergeCell ref="D59:D61"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="B36:B48"/>
-    <mergeCell ref="D36:D40"/>
-    <mergeCell ref="D41:D43"/>
-    <mergeCell ref="D44:D48"/>
-    <mergeCell ref="B49:B54"/>
-    <mergeCell ref="D49:D51"/>
-    <mergeCell ref="B63:G63"/>
-    <mergeCell ref="B65:L65"/>
-    <mergeCell ref="B66:L68"/>
-    <mergeCell ref="B69:F69"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="G5:G6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D52:D54"/>
-    <mergeCell ref="B18:B35"/>
-    <mergeCell ref="D18:D22"/>
-    <mergeCell ref="D23:D27"/>
-    <mergeCell ref="B7:B17"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="D9:D13"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="D28:D30"/>
+    <mergeCell ref="D31:D35"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="E9:E13"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="E16:E17"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>